<commit_message>
cap nhat Internet, CloudinaryService
</commit_message>
<xml_diff>
--- a/Bar Management/Templates/MonAnExcel.xlsx
+++ b/Bar Management/Templates/MonAnExcel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="47">
   <si>
     <t>Danh sách món ăn</t>
   </si>
@@ -40,6 +40,123 @@
   </si>
   <si>
     <t>Mô tả</t>
+  </si>
+  <si>
+    <t>Margarita</t>
+  </si>
+  <si>
+    <t>Đồ Uống Nóng</t>
+  </si>
+  <si>
+    <t>Còn</t>
+  </si>
+  <si>
+    <t>Margarita cổ điển với một chút chanh.</t>
+  </si>
+  <si>
+    <t>Chicken Wings</t>
+  </si>
+  <si>
+    <t>Rượu Vang</t>
+  </si>
+  <si>
+    <t>Cánh gà cay nồng.</t>
+  </si>
+  <si>
+    <t>Vegetarian Pizza</t>
+  </si>
+  <si>
+    <t>Đồ Uống Lạnh</t>
+  </si>
+  <si>
+    <t>Pizza chay ngon với rau sống tươi.</t>
+  </si>
+  <si>
+    <t>Seafood Pasta</t>
+  </si>
+  <si>
+    <t>Mì hải sản phong cách Ý với tỏi và thảo mộc.gg</t>
+  </si>
+  <si>
+    <t>Chocolate Martini</t>
+  </si>
+  <si>
+    <t>Nước Ép Trái Cây</t>
+  </si>
+  <si>
+    <t>Beef Tacos</t>
+  </si>
+  <si>
+    <t>Tacos bò thơm ngon với salsa và guacamole.</t>
+  </si>
+  <si>
+    <t>Caprese Salad</t>
+  </si>
+  <si>
+    <t>Salad Caprese cổ điển với cà chua và phô mai tươi.</t>
+  </si>
+  <si>
+    <t>Nước Chuối</t>
+  </si>
+  <si>
+    <t>Hết</t>
+  </si>
+  <si>
+    <t>Bia Hà Nội</t>
+  </si>
+  <si>
+    <t>Bia</t>
+  </si>
+  <si>
+    <t>Mật ong</t>
+  </si>
+  <si>
+    <t>mật ong vị cà chua</t>
+  </si>
+  <si>
+    <t>Shrimp Scampi</t>
+  </si>
+  <si>
+    <t>Shrimp scampi với bơ tỏi và gừng.</t>
+  </si>
+  <si>
+    <t>Nachos Supreme</t>
+  </si>
+  <si>
+    <t>Sua chua</t>
+  </si>
+  <si>
+    <t>do lanh</t>
+  </si>
+  <si>
+    <t>Them mon an</t>
+  </si>
+  <si>
+    <t>Them mon an moi</t>
+  </si>
+  <si>
+    <t>ssdsddscss</t>
+  </si>
+  <si>
+    <t>sfdsfffdfsfee</t>
+  </si>
+  <si>
+    <t>dfsdfdsfgg</t>
+  </si>
+  <si>
+    <t>fdsfdsf32432</t>
+  </si>
+  <si>
+    <t>rtertre</t>
+  </si>
+  <si>
+    <t>fdfdsf</t>
+  </si>
+  <si>
+    <t>efertre</t>
+  </si>
+  <si>
+    <t>gdfsgdsf</t>
   </si>
 </sst>
 </file>
@@ -687,7 +804,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -695,7 +812,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1015,10 +1137,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:L7"/>
+      <selection activeCell="A26" sqref="A26:F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1076,12 +1198,24 @@
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4">
+        <v>180000</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -1090,12 +1224,24 @@
       <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="4">
+        <v>240003</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -1104,12 +1250,24 @@
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="4">
+        <v>312000</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -1118,12 +1276,24 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4">
+        <v>384000</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -1132,11 +1302,21 @@
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="4">
+        <v>4444</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="F7" s="3"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -1146,148 +1326,522 @@
       <c r="L7" s="2"/>
     </row>
     <row r="8" ht="17" customHeight="1" spans="1:6">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="4">
+        <v>252003</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="4">
+        <v>168000</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="4">
+        <v>168000</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4">
+        <v>168000</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="4">
+        <v>168000</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="4">
+        <v>168000</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="4">
+        <v>168000</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="A15" s="3">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="4">
+        <v>10000</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="4">
+        <v>30000</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="4">
+        <v>6000</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="A18" s="3">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="4">
+        <v>355203</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="A19" s="3">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="4">
+        <v>252001</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+      <c r="A20" s="3">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="4">
+        <v>271201</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="A21" s="3">
+        <v>19</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="4">
+        <v>10000</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="A22" s="3">
+        <v>20</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="4">
+        <v>10000</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
+      <c r="A23" s="3">
+        <v>21</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="4">
+        <v>23000</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="A24" s="3">
+        <v>22</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="4">
+        <v>10000</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="A25" s="3">
+        <v>23</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="4">
+        <v>444444</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="3">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="4">
+        <v>33243</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="3">
+        <v>25</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="4">
+        <v>4444</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="3">
+        <v>26</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="4">
+        <v>455</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="3">
+        <v>27</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="4">
+        <v>455</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="3">
+        <v>28</v>
+      </c>
+      <c r="B30" s="3">
+        <v>34324</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="4">
+        <v>444</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="3">
+        <v>29</v>
+      </c>
+      <c r="B31" s="3">
+        <v>34324</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="4">
+        <v>444</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="3">
+        <v>30</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="4">
+        <v>3333</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="3">
+        <v>31</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="4">
+        <v>6456546</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="3">
+        <v>32</v>
+      </c>
+      <c r="B34" s="3">
+        <v>44</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="4">
+        <v>555</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Tim kiem loc du lieu cua Form Food
</commit_message>
<xml_diff>
--- a/Bar Management/Templates/MonAnExcel.xlsx
+++ b/Bar Management/Templates/MonAnExcel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Danh sách món ăn</t>
   </si>
@@ -30,133 +30,16 @@
     <t>Tên món ăn</t>
   </si>
   <si>
-    <t>Loại món ăn</t>
+    <t>Tên loại</t>
   </si>
   <si>
-    <t xml:space="preserve">Giá </t>
+    <t>Giá</t>
   </si>
   <si>
     <t>Trạng thái</t>
   </si>
   <si>
     <t>Mô tả</t>
-  </si>
-  <si>
-    <t>Margarita</t>
-  </si>
-  <si>
-    <t>Đồ Uống Nóng</t>
-  </si>
-  <si>
-    <t>Còn</t>
-  </si>
-  <si>
-    <t>Margarita cổ điển với một chút chanh.</t>
-  </si>
-  <si>
-    <t>Chicken Wings</t>
-  </si>
-  <si>
-    <t>Rượu Vang</t>
-  </si>
-  <si>
-    <t>Cánh gà cay nồng.</t>
-  </si>
-  <si>
-    <t>Vegetarian Pizza</t>
-  </si>
-  <si>
-    <t>Đồ Uống Lạnh</t>
-  </si>
-  <si>
-    <t>Pizza chay ngon với rau sống tươi.</t>
-  </si>
-  <si>
-    <t>Seafood Pasta</t>
-  </si>
-  <si>
-    <t>Mì hải sản phong cách Ý với tỏi và thảo mộc.gg</t>
-  </si>
-  <si>
-    <t>Chocolate Martini</t>
-  </si>
-  <si>
-    <t>Nước Ép Trái Cây</t>
-  </si>
-  <si>
-    <t>Beef Tacos</t>
-  </si>
-  <si>
-    <t>Tacos bò thơm ngon với salsa và guacamole.</t>
-  </si>
-  <si>
-    <t>Caprese Salad</t>
-  </si>
-  <si>
-    <t>Salad Caprese cổ điển với cà chua và phô mai tươi.</t>
-  </si>
-  <si>
-    <t>Nước Chuối</t>
-  </si>
-  <si>
-    <t>Hết</t>
-  </si>
-  <si>
-    <t>Bia Hà Nội</t>
-  </si>
-  <si>
-    <t>Bia</t>
-  </si>
-  <si>
-    <t>Mật ong</t>
-  </si>
-  <si>
-    <t>mật ong vị cà chua</t>
-  </si>
-  <si>
-    <t>Shrimp Scampi</t>
-  </si>
-  <si>
-    <t>Shrimp scampi với bơ tỏi và gừng.</t>
-  </si>
-  <si>
-    <t>Nachos Supreme</t>
-  </si>
-  <si>
-    <t>Sua chua</t>
-  </si>
-  <si>
-    <t>do lanh</t>
-  </si>
-  <si>
-    <t>Them mon an</t>
-  </si>
-  <si>
-    <t>Them mon an moi</t>
-  </si>
-  <si>
-    <t>ssdsddscss</t>
-  </si>
-  <si>
-    <t>sfdsfffdfsfee</t>
-  </si>
-  <si>
-    <t>dfsdfdsfgg</t>
-  </si>
-  <si>
-    <t>fdsfdsf32432</t>
-  </si>
-  <si>
-    <t>rtertre</t>
-  </si>
-  <si>
-    <t>fdfdsf</t>
-  </si>
-  <si>
-    <t>efertre</t>
-  </si>
-  <si>
-    <t>gdfsgdsf</t>
   </si>
 </sst>
 </file>
@@ -1140,7 +1023,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:F35"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1198,24 +1081,12 @@
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="4">
-        <v>180000</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -1224,24 +1095,12 @@
       <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="3">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="4">
-        <v>240003</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -1250,24 +1109,12 @@
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="3">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="4">
-        <v>312000</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -1276,24 +1123,12 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="3">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="4">
-        <v>384000</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -1302,21 +1137,11 @@
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="3">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="4">
-        <v>4444</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -1326,513 +1151,219 @@
       <c r="L7" s="2"/>
     </row>
     <row r="8" ht="17" customHeight="1" spans="1:6">
-      <c r="A8" s="3">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="4">
-        <v>252003</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="3">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="4">
-        <v>168000</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="3">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="4">
-        <v>168000</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="3">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="4">
-        <v>168000</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="3">
-        <v>10</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="4">
-        <v>168000</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="3">
-        <v>11</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="4">
-        <v>168000</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="3">
-        <v>12</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="4">
-        <v>168000</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="3">
-        <v>13</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="4">
-        <v>10000</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="3">
-        <v>14</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="4">
-        <v>30000</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="3">
-        <v>15</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="4">
-        <v>6000</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>31</v>
-      </c>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="3">
-        <v>16</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="4">
-        <v>355203</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="3">
-        <v>17</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="4">
-        <v>252001</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="3">
-        <v>18</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="4">
-        <v>271201</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="3">
-        <v>19</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="4">
-        <v>10000</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="3">
-        <v>20</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="4">
-        <v>10000</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="3">
-        <v>21</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="4">
-        <v>23000</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="3">
-        <v>22</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="4">
-        <v>10000</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="3">
-        <v>23</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="4">
-        <v>444444</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="3">
-        <v>24</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="4">
-        <v>33243</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="3">
-        <v>25</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="4">
-        <v>4444</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="3">
-        <v>26</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" s="4">
-        <v>455</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="3">
-        <v>27</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="4">
-        <v>455</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="3">
-        <v>28</v>
-      </c>
-      <c r="B30" s="3">
-        <v>34324</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="4">
-        <v>444</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="3">
-        <v>29</v>
-      </c>
-      <c r="B31" s="3">
-        <v>34324</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31" s="4">
-        <v>444</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="3">
-        <v>30</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="4">
-        <v>3333</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="3">
-        <v>31</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="4">
-        <v>6456546</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="3">
-        <v>32</v>
-      </c>
-      <c r="B34" s="3">
-        <v>44</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D34" s="4">
-        <v>555</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
     <row r="35" spans="1:6">

</xml_diff>